<commit_message>
Test: Excel update at
</commit_message>
<xml_diff>
--- a/lancamentos_campanhas_2026.xlsx
+++ b/lancamentos_campanhas_2026.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olliemeu-my.sharepoint.com/personal/breno_lima_meuollie_com_br/Documents/growth_lifecycle/site_calendar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olliemeu-my.sharepoint.com/personal/breno_lima_meuollie_com_br/Documents/growth_lifecycle/site_calendar/calendar-view-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_3505C0EE594E8E3E6D4B4494502D1E7DC9785EB1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B986EAE4-3622-4067-B0F0-0F1C15557629}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_3505C0EE594E8E3E6D4B4494502D1E7DC9785EB1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{019C08DB-9571-48D6-B509-0937EB50A8D0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="62">
   <si>
     <t>Data</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Ainda deve ser validado</t>
+  </si>
+  <si>
+    <t>Previsão</t>
   </si>
 </sst>
 </file>
@@ -600,10 +603,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="A31" sqref="A31:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1269,6 +1272,52 @@
       </c>
       <c r="G30" s="3" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>46194</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>46195</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>